<commit_message>
Fixes to Reporting function
</commit_message>
<xml_diff>
--- a/reports/reports/strategy_results.xlsx
+++ b/reports/reports/strategy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>timestamp</t>
   </si>
@@ -41,11 +41,73 @@
   </si>
   <si>
     <t>improved_sma_windows</t>
+  </si>
+  <si>
+    <t>orig_sharpe</t>
+  </si>
+  <si>
+    <t>orig_n_trades</t>
+  </si>
+  <si>
+    <t>orig_commission</t>
+  </si>
+  <si>
+    <t>orig_initial_capital</t>
+  </si>
+  <si>
+    <t>orig_final_capital</t>
+  </si>
+  <si>
+    <t>improved_sharpe</t>
+  </si>
+  <si>
+    <t>improved_n_trades</t>
+  </si>
+  <si>
+    <t>improved_commission</t>
+  </si>
+  <si>
+    <t>improved_initial_capital</t>
+  </si>
+  <si>
+    <t>improved_final_capital</t>
+  </si>
+  <si>
+    <t>orig_pct_diff_entry_threshold_pct</t>
+  </si>
+  <si>
+    <t>orig_pct_diff_exit_threshold_pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="### 1️⃣ Explanation: 
+Mean Reversion Strategy for TSLA: Buy when 5-min Close price falls below Lower Bollinger Band (2 std devs), Sell when above Upper Bollinger Band, otherwise Hold.
+### 2️⃣ `add_signal` Function
+</t>
   </si>
   <si>
     <t xml:space="preserve">content="### 1️⃣ Explanation: 
 Mean Reversion Strategy for TSLA: Buy when 5-min Close price falls below its 20-period Simple Moving Average (SMA) by more than 1.5%, Sell when it rises above by more than 1.5%, otherwise Hold.
 ### 2️⃣ `add_signal` Function
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    # Calculate Simple Moving Average (SMA) over 20 periods (100 minutes)
+    df['sma'] = df['Close'].rolling(window=20).mean()
+    # Calculate Standard Deviation over 20 periods
+    df['std_dev'] = df['Close'].rolling(window=20).std()
+    # Define Bollinger Bands (2 standard deviations from SMA)
+    df['lower_bb'] = df['sma'] - 2 * df['std_dev']
+    df['upper_bb'] = df['sma'] + 2 * df['std_dev']
+    # Initialize signals array with Hold (0) by default
+    signals = np.zeros(len(df))
+    # Assign Buy (1) when Close price falls below Lower Bollinger Band
+    signals[(df['Close'] &lt; df['lower_bb'])] = 1
+    # Assign Sell (-1) when Close price rises above Upper Bollinger Band
+    signals[(df['Close'] &gt; df['upper_bb'])] = -1
+    # Add signals to the original DataFrame
+    df['signal'] = signals
 </t>
   </si>
   <si>
@@ -57,25 +119,71 @@
     df['pct_diff'] = ((df['Close'] - df['sma_20']) / df['sma_20']) * 100
     # Initialize signal column with Hold (0) as default
     df['signal'] = 0
-    # Set Buy (1) when Close is more than 1.5% below SMA
+    # Set Buy (1) signal when Close is more than 1.5% below SMA
     df.loc[df['pct_diff'] &lt; -1.5, 'signal'] = 1
-    # Set Sell (-1) when Close is more than 1.5% above SMA
+    # Set Sell (-1) signal when Close is more than 1.5% above SMA
     df.loc[df['pct_diff'] &gt; 1.5, 'signal'] = -1
 </t>
   </si>
   <si>
     <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+Based on the provided backtest results, the strategy's weaknesses are:
+1. **Negative Total Return**: The strategy resulted in a loss of -0.83% over the 5-day period, indicating that the current buy/sell logic is not effective.
+2. **High Max Drawdown**: A 0.60% max drawdown in a short period suggests that the strategy is prone to significant short-term losses.
+3. **Low Sharpe Ratio**: A Sharpe Ratio of -0.71 implies that the strategy's returns are largely driven by risk rather than alpha.
+4. **Frequent Trading**: 8 trades in 5 days may lead to high transaction costs, as evidenced by the $80 fee cost.
+To address these weaknesses, the revised strategy will focus on:
+1. **Improving risk management**: Reduce exposure to large losses.
+2. **Enhancing return potential**: Identify more effective entry/exit points.
+3. **Decreasing trading frequency**: Minimize transaction costs.
+**Revised Strategy: "Mean Reversion with Volatility Guard"**
+This strategy combines mean reversion with a volatility-based filter to reduce risk and improve returns.
+**Python Code**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
 Based on the provided strategy and backtest results, the following weaknesses and potential improvements are identified:
-1. **Overly Simple Entry/Exit Logic**: The strategy relies solely on a percentage difference between the Close price and a 20-period SMA, which might not capture more nuanced market dynamics.
-2. **High Frequency of Trades**: 8 trades in 5 trading days (approximately 1.6 trades per day) may lead to increased transaction costs, potentially eating into profits.
-3. **Limited Risk Management**: No explicit stop-loss or position sizing mechanism is implemented, which could exacerbate losses during adverse market movements.
-4. **Low Profitability**: A -0.06% total return over 5 trading days indicates room for improvement in the strategy's profitability.
-**Revised Strategy: "Dual SMA with Volatility-Based Position Sizing"**
-**Brief Explanation:**
+1. **Overly Simple Logic**: The strategy relies solely on the percentage difference between the Close price and a 20-period SMA, which might not capture more nuanced market behaviors.
+2. **High Trade Frequency**: With 8 trades over 5 trading days (approximately 1 trade per day), transaction costs (e.g., the $80 fee) might erode profits. Reducing trade frequency while maintaining or improving profitability is desirable.
+3. **Limited Risk Management**: The strategy lacks explicit risk management techniques, such as position sizing based on volatility or maximum allowable loss per trade.
+4. **Low Profitability**: The -0.06% total return over 5 days is underwhelming, suggesting the need for a more effective entry/exit logic.
+**Revised Strategy: "Improved SMA Crossover with Volatility-Based Position Sizing"**
+**Brief Explanation**:
 This revised strategy aims to enhance profitability and reduce volatility by:
-* Utilizing a dual SMA approach to generate more informed entry/exit signals.
-* Incorporating a basic volatility-based position sizing mechanism to manage risk.
-**Revised Python Strategy Function:**
+* Introducing a dual SMA crossover system for more informed entry/exit decisions.
+* Incorporating a basic form of risk management through volatility-based position sizing (though, for simplicity, this aspect is simulated by adjusting the signal strength rather than actual position sizing, as the latter would require additional portfolio management logic not specified in the original task).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import numpy as np
+import pandas as pd
+def add_signal(df):
+    """
+    Adds a 'signal' column to the input DataFrame based on a mean reversion strategy with volatility guard.
+    """
+    # Calculate Short-Term Simple Moving Average (10 periods, 50 minutes)
+    df['sma_short'] = df['Close'].rolling(window=10).mean()
+    # Calculate Long-Term Simple Moving Average (30 periods, 150 minutes)
+    df['sma_long'] = df['Close'].rolling(window=30).mean()
+    # Calculate Standard Deviation over 20 periods (100 minutes)
+    df['std_dev'] = df['Close'].rolling(window=20).std()
+    # Volatility Guard: only trade when std_dev is below the 20-period average std_dev
+    avg_std_dev = df['std_dev'].rolling(window=20).mean()
+    volatility_guard = df['std_dev'] &lt; avg_std_dev
+    # Mean Reversion Logic
+    # Buy when Close price falls below SMA (short) and SMA (short) is above SMA (long)
+    buy_logic = (df['Close'] &lt; df['sma_short']) &amp; (df['sma_short'] &gt; df['sma_long']) &amp; volatility_guard
+    # Sell when Close price rises above SMA (short) and SMA (short) is below SMA (long)
+    sell_logic = (df['Close'] &gt; df['sma_short']) &amp; (df['sma_short'] &lt; df['sma_long']) &amp; volatility_guard
+    # Initialize signals array with Hold (0) by default
+    signals = np.zeros(len(df), dtype=int)
+    # Assign Buy (1) and Sell (-1) signals
+    signals[buy_logic] = 1
+    signals[sell_logic] = -1
+    # Add signals to the original DataFrame, ensuring same index
+    df["signal"] = pd.Series(signals, index=df.index)
 </t>
   </si>
   <si>
@@ -84,33 +192,25 @@
 import numpy as np
 def add_signal(df):
     """
-    Adds a 'signal' column to the input DataFrame based on a dual SMA strategy
-    with volatility-based position sizing.
+    Revised strategy adding a 'signal' column to the DataFrame.
+    Dual SMA Crossover with Simulated Volatility-Based Signal Strength
     """
-    # Calculate Short and Long Simple Moving Averages (SMA)
+    # Calculate Short and Long Simple Moving Averages
     df['sma_short'] = df['Close'].rolling(window=10).mean()
-    df['sma_long'] = df['Close'].rolling(window=20).mean()
-    # Calculate Historical Volatility (HV) for position sizing
-    df['hv'] = df['Close'].rolling(window=20).std() * np.sqrt(5)  # 5-minute bars, scaled to daily HV
+    df['sma_long'] = df['Close'].rolling(window=30).mean()
+    # Calculate Volatility (Simple Measure: Close Price Standard Deviation over 20 periods)
+    df['volatility'] = df['Close'].rolling(window=20).std()
     # Initialize signal column with Hold (0) as default
-    df['signal'] = pd.Series(0, index=df.index)
-    # Set Buy (1) when Short SMA crosses above Long SMA and HV is below 2%
-    buy_conditions = (df['sma_short'] &gt; df['sma_long']) &amp; (df['hv'] &lt; df['Close'] * 0.02)
-    df.loc[buy_conditions, 'signal'] = 1
-    # Set Sell (-1) when Short SMA crosses below Long SMA or HV exceeds 3%
-    sell_conditions = (df['sma_short'] &lt; df['sma_long']) | (df['hv'] &gt; df['Close'] * 0.03)
-    df.loc[sell_conditions, 'signal'] = -1
-    # Basic Volatility-Based Position Sizing (example: reduce position size with increasing HV)
-    df['position_size'] = pd.Series(1.0, index=df.index)  # default 100% position size
-    df.loc[df['hv'] &gt; df['Close'] * 0.025, 'position_size'] = 0.75  # reduce to 75% if HV &gt; 2.5%
-    df.loc[df['hv'] &gt; df['Close'] * 0.035, 'position_size'] = 0.5   # reduce to 50% if HV &gt; 3.5%
+    df['signal'] = 0
+    # Identify Buy and Sell Crossover Points
+    buy_crossover = (df['sma_short'] &gt; df['sma_long']) &amp; (df['sma_short'].shift(1) &lt;= df['sma_long'].shift(1))
+    sell_crossover = (df['sma_short'] &lt; df['sma_long']) &amp; (df['sma_short'].shift(1) &gt;= df['sma_long'].shift(1))
+    # Assign Buy (1) and Sell (-1) Signals Based on Crossover, Adjusting Strength by Volatility
+    df.loc[buy_crossover, 'signal'] = 1 / (1 + df['volatility'] / df['Close'])  # Simulated position sizing based on volatility
+    df.loc[sell_crossover, 'signal'] = -1 / (1 + df['volatility'] / df['Close'])
+    # Ensure signal Series uses the same index as df
+    df['signal'] = pd.Series(df['signal'].values, index=df.index)
 </t>
-  </si>
-  <si>
-    <t>[20]</t>
-  </si>
-  <si>
-    <t>[10, 20, 20]</t>
   </si>
 </sst>
 </file>
@@ -472,13 +572,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,34 +606,141 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:21">
       <c r="A2" s="2">
-        <v>45787.59256878892</v>
+        <v>45787.60035719907</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2">
+        <v>-0.71</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>80</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="O2">
+        <v>-29.21</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2">
+        <v>70</v>
+      </c>
+      <c r="R2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
+      <c r="S2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2">
+        <v>45787.64977077832</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3">
+        <v>12.31</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>80</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>-22.27</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>59.67</v>
+      </c>
+      <c r="R3">
+        <v>10</v>
+      </c>
+      <c r="S3">
+        <v>9</v>
+      </c>
+      <c r="T3">
         <v>1.5</v>
       </c>
-      <c r="H2">
+      <c r="U3">
         <v>1.5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model change and prompt reversion
</commit_message>
<xml_diff>
--- a/reports/reports/strategy_results.xlsx
+++ b/reports/reports/strategy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>timestamp</t>
   </si>
@@ -77,6 +77,27 @@
   </si>
   <si>
     <t>orig_pct_diff_exit_threshold_pct</t>
+  </si>
+  <si>
+    <t>orig_return_pct</t>
+  </si>
+  <si>
+    <t>orig_max_drawdown_pct</t>
+  </si>
+  <si>
+    <t>improved_return_pct</t>
+  </si>
+  <si>
+    <t>improved_max_drawdown_pct</t>
+  </si>
+  <si>
+    <t>improved_sma_short_window</t>
+  </si>
+  <si>
+    <t>improved_sma_long_window</t>
+  </si>
+  <si>
+    <t>improved_bb_window</t>
   </si>
   <si>
     <t xml:space="preserve">content="### 1️⃣ Explanation: 
@@ -88,6 +109,10 @@
     <t xml:space="preserve">content="### 1️⃣ Explanation: 
 Mean Reversion Strategy for TSLA: Buy when 5-min Close price falls below its 20-period Simple Moving Average (SMA) by more than 1.5%, Sell when it rises above by more than 1.5%, otherwise Hold.
 ### 2️⃣ `add_signal` Function
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='Explanation: Simple Moving Average Crossover Strategy for TSLA with 50-period short MA and 200-period long MA.
 </t>
   </si>
   <si>
@@ -126,6 +151,36 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df["signal"] = 0
+    short_window = 50
+    long_window = 200
+    df["short_ma"] = df["Close"].rolling(window=short_window).mean()
+    df["long_ma"] = df["Close"].rolling(window=long_window).mean()
+    buy_mask = (df["short_ma"] &gt; df["long_ma"]) &amp; (df["short_ma"].shift(1) &lt;= df["long_ma"].shift(1))
+    sell_mask = (df["short_ma"] &lt; df["long_ma"]) &amp; (df["short_ma"].shift(1) &gt;= df["long_ma"].shift(1))
+    df.loc[buy_mask, "signal"] = 1
+    df.loc[sell_mask, "signal"] = -1
+    df.drop(columns=["short_ma", "long_ma"], inplace=True)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    # Calculate Simple Moving Average (SMA) over 20 periods
+    df['sma_20'] = df['Close'].rolling(window=20).mean()
+    # Calculate percentage difference between Close and SMA
+    df['pct_diff'] = ((df['Close'] - df['sma_20']) / df['sma_20']) * 100
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = 0
+    # Set Buy (1) when Close is more than 1.5% below SMA
+    df.loc[df['pct_diff'] &lt; -1.5, 'signal'] = 1
+    # Set Sell (-1) when Close is more than 1.5% above SMA
+    df.loc[df['pct_diff'] &gt; 1.5, 'signal'] = -1
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
 Based on the provided backtest results, the strategy's weaknesses are:
 1. **Negative Total Return**: The strategy resulted in a loss of -0.83% over the 5-day period, indicating that the current buy/sell logic is not effective.
@@ -153,6 +208,51 @@
 This revised strategy aims to enhance profitability and reduce volatility by:
 * Introducing a dual SMA crossover system for more informed entry/exit decisions.
 * Incorporating a basic form of risk management through volatility-based position sizing (though, for simplicity, this aspect is simulated by adjusting the signal strength rather than actual position sizing, as the latter would require additional portfolio management logic not specified in the original task).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+1. **Lack of Trades**: The backtest results show zero trades, indicating the strategy's conditions are too restrictive or not met during the 5-day period. This could be due to the long window period (200) being too large for a 5-day dataset, resulting in no crossovers.
+2. **Insufficient Risk Management**: The strategy doesn't incorporate any risk management techniques, such as position sizing, stop-loss, or take-profit levels.
+3. **Over-Simplistic Entry/Exit Logic**: The strategy relies solely on a simple moving average crossover, which might not be effective in capturing more complex market dynamics.
+**Revised Strategy: "Dual-Threshold MA Crossover with Risk Management"**
+**Brief Explanation**:
+This revised strategy aims to enhance profitability and reduce volatility by:
+* Introducing dual thresholds for MA crossovers to filter out weaker signals.
+* Implementing a basic risk management system using a fixed fractional position sizing.
+* Reducing the long window period to increase the strategy's responsiveness to the 5-day dataset.
+**Revised Python Strategy Function**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+1. **Lack of Trades**: The backtest results show zero trades, indicating the strategy's conditions are too restrictive or not triggered during the tested period.
+2. **Simple Moving Averages (MA)**: Using only two simple MAs might not capture more nuanced market trends. 
+3. **No Risk Management**: The strategy doesn't incorporate position sizing, stop-loss, or take-profit mechanisms, which are crucial for managing volatility and maximizing profitability.
+4. **No Confirmation from Other Indicators**: Relying solely on MA crossovers can lead to false signals. Adding confirmation from other indicators can enhance signal reliability.
+**Revised Strategy: Enhanced MA Crossover with Risk Management and Confirmation**
+**Brief Explanation**:
+This revised strategy enhances the original by:
+- Incorporating a **short-term** and **medium-term** MA for more nuanced trend detection.
+- Adding **Relative Strength Index (RSI)** as a confirmation indicator to reduce false signals.
+- Implementing **basic position sizing** based on the strategy's equity (though for simplicity, we won't adjust trade sizes here; in a real scenario, you'd integrate this with your backtesting framework's capabilities).
+- Introducing **stop-loss** and **take-profit** levels based on Average True Range (ATR) to manage risk.
+**Revised Python Strategy Function**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+Based on the provided strategy and backtest results, the following weaknesses and potential improvements are identified:
+1. **Overly Simple Entry/Exit Logic**: The strategy relies solely on a percentage difference between the Close price and a 20-period SMA, which might not capture more nuanced market dynamics.
+2. **High Frequency of Trades**: 8 trades in 5 trading days (approximately 1.6 trades per day) may lead to increased transaction costs, potentially eating into profits.
+3. **Limited Risk Management**: No explicit stop-loss or position sizing mechanism is implemented, which could exacerbate losses during adverse market movements.
+4. **Low Profitability**: A -0.06% total return over 5 trading days indicates room for improvement in the strategy's profitability.
+**Revised Strategy: "Dual SMA with Volatility-Based Position Sizing"**
+**Brief Explanation:**
+This revised strategy aims to enhance profitability and reduce volatility by:
+* Utilizing a dual SMA approach to generate more informed entry/exit signals.
+* Incorporating a basic volatility-based position sizing mechanism to manage risk.
+**Revised Python Strategy Function:**
 </t>
   </si>
   <si>
@@ -210,6 +310,118 @@
     df.loc[sell_crossover, 'signal'] = -1 / (1 + df['volatility'] / df['Close'])
     # Ensure signal Series uses the same index as df
     df['signal'] = pd.Series(df['signal'].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Modifies the input DataFrame to add a 'signal' column based on a dual-threshold MA crossover strategy
+    with basic risk management.
+    """
+    # Risk Management Parameters
+    risk_fraction = 0.02  # 2% of capital per trade
+    stop_loss_pct = 0.05  # 5% stop-loss
+    take_profit_pct = 0.10  # 10% take-profit
+    # Moving Average Windows
+    short_window = 20
+    long_window = 50
+    # Calculate Moving Averages
+    df["short_ma"] = df["Close"].rolling(window=short_window).mean()
+    df["long_ma"] = df["Close"].rolling(window=long_window).mean()
+    # Dual Thresholds for MA Crossover
+    threshold_buy = 0.005  # 0.5% above long MA to buy
+    threshold_sell = -0.005  # 0.5% below long MA to sell
+    # Generate Signals
+    buy_mask = ((df["short_ma"] &gt; (1 + threshold_buy) * df["long_ma"]) &amp;
+                (df["short_ma"].shift(1) &lt;= df["long_ma"].shift(1)))
+    sell_mask = ((df["short_ma"] &lt; (1 + threshold_sell) * df["long_ma"]) &amp;
+                 (df["short_ma"].shift(1) &gt;= df["long_ma"].shift(1)))
+    # Assign Signals with Risk Management
+    signal_array = np.zeros(len(df))
+    signal_array[buy_mask] = 1
+    signal_array[sell_mask] = -1
+    # Basic Position Sizing (Fixed Fractional)
+    df["position_size"] = risk_fraction * 10000 / df["Close"]  # Assuming $10,000 initial capital
+    # Stop-Loss and Take-Profit Levels (for further development)
+    # df["stop_loss"] = df["Close"] * (1 - stop_loss_pct)
+    # df["take_profit"] = df["Close"] * (1 + take_profit_pct)
+    # Assign Signal Column
+    df["signal"] = pd.Series(signal_array, index=df.index)
+    # Clean Up
+    df.drop(columns=["short_ma", "long_ma"], inplace=True)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Parameters
+    short_window = 20
+    medium_window = 50
+    long_window = 200
+    rsi_window = 14
+    atr_window = 14
+    stop_loss_atr_multiple = 2
+    take_profit_atr_multiple = 3
+    # Calculate Indicators
+    df["short_ma"] = df["Close"].rolling(window=short_window).mean()
+    df["medium_ma"] = df["Close"].rolling(window=medium_window).mean()
+    df["long_ma"] = df["Close"].rolling(window=long_window).mean()
+    delta = df["Close"].diff(1)
+    up, down = delta.copy(), delta.copy()
+    up[up &lt; 0] = 0
+    down[down &gt; 0] = 0
+    roll_up = up.rolling(window=rsi_window).mean()
+    roll_down = down.rolling(window=rsi_window).mean().abs()
+    RS = roll_up / roll_down
+    df["RSI"] = 100.0 - (100.0 / (1.0 + RS))
+    df["atr"] = df['High'].rolling(window=atr_window).max() - df['Low'].rolling(window=atr_window).min()
+    # Signal Generation
+    df["signal"] = 0
+    # Buy Signal: Short MA &gt; Medium MA, and RSI &lt; 70 (not overbought)
+    buy_mask = (df["short_ma"] &gt; df["medium_ma"]) &amp; (df["short_ma"].shift(1) &lt;= df["medium_ma"].shift(1)) &amp; (df["RSI"] &lt; 70)
+    # Sell Signal: Short MA &lt; Medium MA, and RSI &gt; 30 (not oversold)
+    sell_mask = (df["short_ma"] &lt; df["medium_ma"]) &amp; (df["short_ma"].shift(1) &gt;= df["medium_ma"].shift(1)) &amp; (df["RSI"] &gt; 30)
+    df.loc[buy_mask, "signal"] = 1
+    df.loc[sell_mask, "signal"] = -1
+    # Basic Risk Management (for demonstration; integrate with backtester for dynamic sizing)
+    df["stop_loss"] = df["Close"] - (df["atr"] * stop_loss_atr_multiple)
+    df["take_profit"] = df["Close"] + (df["atr"] * take_profit_atr_multiple)
+    # Cleanup
+    df.drop(columns=["short_ma", "medium_ma", "long_ma"], inplace=True)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the input DataFrame based on a dual SMA strategy
+    with volatility-based position sizing.
+    """
+    # Calculate Short and Long Simple Moving Averages (SMA)
+    df['sma_short'] = df['Close'].rolling(window=10).mean()
+    df['sma_long'] = df['Close'].rolling(window=20).mean()
+    # Calculate Historical Volatility (HV) as a measure of risk
+    df['hv'] = df['Close'].rolling(window=20).std() * np.sqrt(5*60)  # Adjust for 5-minute bars
+    # Initialize signal and position size columns
+    df['signal'] = 0
+    df['position_size'] = 0.0
+    # Generate Buy (1) signals when short SMA crosses above long SMA
+    buy_conditions = (df['sma_short'] &gt; df['sma_long']) &amp; (df['sma_short'].shift(1) &lt;= df['sma_long'].shift(1))
+    df.loc[buy_conditions, 'signal'] = 1
+    # Generate Sell (-1) signals when short SMA crosses below long SMA
+    sell_conditions = (df['sma_short'] &lt; df['sma_long']) &amp; (df['sma_short'].shift(1) &gt;= df['sma_long'].shift(1))
+    df.loc[sell_conditions, 'signal'] = -1
+    # Volatility-Based Position Sizing (simplified example)
+    df.loc[df['signal'] != 0, 'position_size'] = pd.Series(10000 / df['hv'], index=df.index)  # Assuming $10,000 initial capital
+    # Ensure signal Series uses the same index as df
+    df["signal"] = pd.Series(df["signal"].values, index=df.index)
 </t>
   </si>
 </sst>
@@ -572,13 +784,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,22 +854,43 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:28">
       <c r="A2" s="2">
         <v>45787.60035719907</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="J2">
         <v>-0.71</v>
@@ -690,21 +923,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:28">
       <c r="A3" s="2">
-        <v>45787.64977077832</v>
+        <v>45787.64977077546</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J3">
         <v>12.31</v>
@@ -741,6 +974,180 @@
       </c>
       <c r="U3">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="2">
+        <v>45787.6773174074</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>10000</v>
+      </c>
+      <c r="N4">
+        <v>10000</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>10000</v>
+      </c>
+      <c r="S4">
+        <v>10000</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="2">
+        <v>45787.68231012731</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>10000</v>
+      </c>
+      <c r="N5">
+        <v>10000</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>10000</v>
+      </c>
+      <c r="S5">
+        <v>10000</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="2">
+        <v>45787.68987413317</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6">
+        <v>12.31</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>80</v>
+      </c>
+      <c r="M6">
+        <v>10000</v>
+      </c>
+      <c r="N6">
+        <v>9994.5</v>
+      </c>
+      <c r="O6">
+        <v>24.69</v>
+      </c>
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6">
+        <v>60</v>
+      </c>
+      <c r="R6">
+        <v>10000</v>
+      </c>
+      <c r="S6">
+        <v>9990.969999999999</v>
+      </c>
+      <c r="V6">
+        <v>-0.06</v>
+      </c>
+      <c r="W6">
+        <v>0.49</v>
+      </c>
+      <c r="X6">
+        <v>-0.09</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>10</v>
+      </c>
+      <c r="AA6">
+        <v>20</v>
+      </c>
+      <c r="AB6">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Readme update with personal details
</commit_message>
<xml_diff>
--- a/reports/reports/strategy_results.xlsx
+++ b/reports/reports/strategy_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>timestamp</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>improved_bb_window</t>
+  </si>
+  <si>
+    <t>orig_sma_short_window</t>
+  </si>
+  <si>
+    <t>orig_sma_long_window</t>
   </si>
   <si>
     <t xml:space="preserve">content="### 1️⃣ Explanation: 
@@ -113,6 +119,22 @@
   </si>
   <si>
     <t xml:space="preserve">content='Explanation: Simple Moving Average Crossover Strategy for TSLA with 50-period short MA and 200-period long MA.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="Explanation: This strategy generates a buy signal when the price is above the 50-period moving average and a sell signal when the price is below the 20-period moving average.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="Explanation: This strategy generates a buy signal when the price is above a short-term moving average and a sell signal when it's below a long-term moving average, with a hold signal otherwise.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="Explanation: This strategy generates a buy signal when the price is above the 20-period moving average, a sell signal when the price is below the 20-period moving average, and a hold signal otherwise.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="Explanation: This strategy generates a buy signal when the short-term moving average (50 periods) crosses above the long-term moving average (200 periods), a sell signal when it crosses below, and a hold signal otherwise.
 </t>
   </si>
   <si>
@@ -181,6 +203,73 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    # Calculate Simple Moving Average (SMA) over 20 periods
+    df['sma'] = df['Close'].rolling(window=20).mean()
+    # Calculate Standard Deviation over 20 periods
+    df['std_dev'] = df['Close'].rolling(window=20).std()
+    # Define Bollinger Bands (2 standard deviations from SMA)
+    df['lower_bb'] = df['sma'] - 2 * df['std_dev']
+    df['upper_bb'] = df['sma'] + 2 * df['std_dev']
+    # Initialize signal column with Hold (0) by default
+    df['signal'] = 0
+    # Generate Buy signal (1) when Close price crosses below Lower BB
+    buy_conditions = (df['Close'] &lt; df['lower_bb']) &amp; (df['Close'].shift(1) &gt;= df['lower_bb'].shift(1))
+    df.loc[buy_conditions, 'signal'] = 1
+    # Generate Sell signal (-1) when Close price crosses above Upper BB
+    sell_conditions = (df['Close'] &gt; df['upper_bb']) &amp; (df['Close'].shift(1) &lt;= df['upper_bb'].shift(1))
+    df.loc[sell_conditions, 'signal'] = -1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df['MA_20'] = df['Close'].rolling(window=20).mean()
+    df['MA_50'] = df['Close'].rolling(window=50).mean()
+    signals = np.where(df['Close'] &gt; df['MA_50'], 1, np.where(df['Close'] &lt; df['MA_20'], -1, 0))
+    df['signal'] = signals
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    df['signal'] = np.where(df['Close'] &gt; df['short_ma'], 1, np.where(df['Close'] &lt; df['long_ma'], -1, 0))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    df['signal'] = np.where(df['Close'] &gt; df['short_ma'], 1, 
+                            np.where(df['Close'] &lt; df['long_ma'], -1, 0))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df['MA_20'] = df['Close'].rolling(window=20).mean()
+    df['signal'] = np.where(df['Close'] &gt; df['MA_20'], 1, np.where(df['Close'] &lt; df['MA_20'], -1, 0))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+def add_signal(df):
+    df['short_ma'] = df['Close'].rolling(window=50).mean()
+    df['long_ma'] = df['Close'].rolling(window=200).mean()
+    df['signal'] = 0
+    df.loc[(df['short_ma'] &gt; df['long_ma']) &amp; (df['short_ma'].shift(1) &lt;= df['long_ma'].shift(1)), 'signal'] = 1
+    df.loc[(df['short_ma'] &lt; df['long_ma']) &amp; (df['short_ma'].shift(1) &gt;= df['long_ma'].shift(1)), 'signal'] = -1
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
 Based on the provided backtest results, the strategy's weaknesses are:
 1. **Negative Total Return**: The strategy resulted in a loss of -0.83% over the 5-day period, indicating that the current buy/sell logic is not effective.
@@ -253,6 +342,171 @@
 * Utilizing a dual SMA approach to generate more informed entry/exit signals.
 * Incorporating a basic volatility-based position sizing mechanism to manage risk.
 **Revised Python Strategy Function:**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+1. **Overly Simplistic Entry/Exit Logic**: The strategy relies solely on the percentage difference between the Close price and a 20-period SMA, which might not capture more nuanced market dynamics.
+2. **Lack of Risk Management**: No explicit stop-loss or position sizing is implemented, potentially leading to significant losses if the market moves adversely.
+3. **Insufficient Filter for False Signals**: The strategy might generate multiple signals in a short period if the price oscillates around the SMA, leading to increased transaction costs.
+4. **No Consideration for Market Context**: The strategy does not account for broader market trends, volatility, or time of day, which could influence trade success.
+**Revised Strategy: "Context-Aware Mean Reversion with Risk Management"**
+**Brief Explanation**:
+This revised strategy enhances the original by incorporating:
+* A **volatility filter** to reduce false signals during high-volatility periods.
+* A **broader market trend filter** to align trades with the overall market direction.
+* **Basic risk management** through position sizing based on the Average True Range (ATR).
+* **Improved entry logic** using a combination of SMA and Bollinger Bands.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+Based on the provided strategy and backtest results, the following weaknesses and potential improvements are identified:
+1. **Overly Simple Entry/Exit Logic**: The strategy relies solely on a percentage difference between the Close price and a 20-period SMA, which might not capture more nuanced market dynamics.
+2. **Lack of Risk Management**: No explicit stop-loss or position sizing is implemented, which could exacerbate losses during periods of high volatility.
+3. **Insufficient Filter for False Signals**: The strategy might generate multiple buy/sell signals in quick succession, leading to increased transaction costs without significant profit improvements.
+4. **Limited Profit Maximization**: There's no mechanism to lock in profits or adjust positions as the market moves in favor of the trade.
+**Revised Strategy: "Improved SMA Crossover with Risk Management"**
+**Brief Explanation:**
+This revised strategy enhances the original by incorporating:
+* A shorter SMA for faster signal generation and a longer SMA for trend confirmation.
+* A volatility-based stop-loss to limit potential losses.
+* A simple profit-taking mechanism to lock in gains.
+* Reduced signal noise by requiring a stronger price move before generating a new signal.
+**Revised Python Strategy Function:**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='**Analysis of Weaknesses and Improvements**
+1. **Over-simplistic entry/exit rules**: The original strategy relies solely on the percentage difference between the Close price and a 20-period SMA, leading to potential whipsaws in volatile markets.
+2. **Lack of risk management**: No consideration is given to position sizing, stop-loss, or take-profit levels, which can exacerbate losses or cap gains.
+3. **Insufficient signal confirmation**: Signals are generated solely based on the SMA deviation without confirming the market's direction or momentum.
+**Revised Strategy: "SMA Momentum Confirmation with Risk Management"**
+**Brief Explanation:**
+This revised strategy aims to enhance profitability and reduce volatility by:
+* Confirming buy/sell signals with a short-term momentum indicator (RSI).
+* Implementing basic risk management through position sizing based on Average True Range (ATR).
+* Maintaining a simple, deterministic, and Pandas/Numpy-only approach.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="**Analysis of Weaknesses and Improvements**
+1. **Low Profitability**: The strategy's -0.82% total return indicates that the current buy/sell logic may not be effective in capturing profitable trades.
+2. **High Frequency of Trades**: 8 trades in 5 trading days (approximately 1.6 trades per day) may lead to increased transaction costs, eating into potential profits.
+3. **Simple Thresholds**: Using fixed 2-standard-deviation Bollinger Bands might not adapt well to changing market volatility.
+4. **No Risk Management**: The strategy lacks position sizing or stop-loss mechanisms to limit potential losses.
+**Revised Strategy: Adaptive Bollinger Bands with Volatility-Based Position Sizing**
+**Brief Explanation:**
+This revised strategy aims to improve profitability and reduce volatility by:
+* Using adaptive Bollinger Bands with a dynamic standard deviation multiplier based on recent market volatility.
+* Implementing a basic risk management system with position sizing based on the Average True Range (ATR).
+**Revised Python Strategy:**
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses two moving averages (MA) with windows of 20 and 50 periods to generate buy and sell signals. The strategy buys when the closing price is above the 50-period MA and sells when the closing price is below the 20-period MA. 
+The weaknesses in this strategy are:
+1. **Lack of Risk Management**: The strategy does not consider any risk management techniques, such as position sizing or stop-loss levels.
+2. **Simple MA Crossover**: The strategy relies solely on the MA crossover, which can lead to whipsaws and false signals in volatile markets.
+3. **No Consideration of Market Conditions**: The strategy does not account for different market conditions, such as trends, ranges, or breakouts.
+4. **Insufficient Parameters**: The strategy uses fixed MA windows, which may not be optimal for all market conditions.
+### Revised Strategy
+To improve the strategy, we can incorporate additional indicators and risk management techniques. Here's a revised strategy that uses the Relative Strength Index (RSI) and Bollinger Bands to generate buy and sell signals.
+**Brief Explanation:**
+The revised strategy uses the RSI to identify overbought and oversold conditions, and Bollinger Bands to determine volatility. It buys when the RSI is oversold and the price is below the lower Bollinger Band, and sells when the RSI is overbought and the price is above the upper Bollinger Band.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the short and long moving averages, without taking into account other factors that might influence the stock price, such as volatility, trends, or momentum.
+*   The strategy uses a fixed window size for the short and long moving averages, which might not be optimal for all market conditions.
+*   The strategy does not have a risk management component, which can lead to large losses if the market moves against the strategy.
+### Revised Strategy
+To address these weaknesses, we can modify the strategy to include additional factors and use more advanced techniques. Here's a revised strategy that uses a combination of moving averages and the Relative Strength Index (RSI) to generate buy and sell signals.
+### Explanation of the Revised Strategy
+The revised strategy uses the following rules to generate buy and sell signals:
+*   Buy signal: When the short moving average crosses above the long moving average and the RSI is below 30 (oversold condition).
+*   Sell signal: When the short moving average crosses below the long moving average and the RSI is above 70 (overbought condition).
+*   Hold signal: When neither of the above conditions is met.
+### Revised Python Strategy Function
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the short and long moving averages, without taking into account other factors that might influence the stock price, such as volatility, trends, or momentum.
+*   The strategy uses a fixed window size for the short and long moving averages, which might not be optimal for all market conditions.
+*   The strategy does not have any risk management mechanisms, such as stop-loss or position sizing, which can help to limit losses and maximize gains.
+### Revised Strategy
+To improve the strategy, we can add a few more features:
+*   Use exponential moving averages (EMAs) instead of simple moving averages (SMAs), as EMAs give more weight to recent prices and can react faster to changes in the market.
+*   Add a momentum indicator, such as the Relative Strength Index (RSI), to help identify overbought and oversold conditions.
+*   Use a risk management mechanism, such as a stop-loss, to limit losses.
+### Revised Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the short and long moving averages, without taking into account other factors that may affect the stock price, such as volatility, trends, or momentum.
+*   The strategy uses a fixed window size for the short and long moving averages, which may not be optimal for all market conditions.
+*   The strategy does not have a risk management component, which can lead to significant losses if the market moves against the strategy.
+### Revised Strategy
+To improve the strategy, we can add a risk management component and consider other factors that may affect the stock price. One possible approach is to use a combination of moving averages and a volatility-based indicator, such as the Average True Range (ATR).
+Here is a revised version of the Python strategy:
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the short and long moving averages, without taking into account other factors that may influence the stock price, such as volatility, trends, or momentum.
+*   The strategy uses a fixed window size for the moving averages, which may not be optimal for all market conditions.
+*   The strategy does not have a risk management component, which can lead to large losses if the strategy is not performing well.
+### Revised Strategy
+To address these weaknesses, we can modify the strategy to include additional factors and use more advanced techniques. Here's a revised strategy that uses a combination of moving averages and the Relative Strength Index (RSI) to generate trading signals.
+The RSI is a momentum indicator that measures the magnitude of recent price changes to determine overbought or oversold conditions. By incorporating the RSI into our strategy, we can avoid buying or selling during periods of high volatility or when the stock is overbought or oversold.
+### Revised Strategy Code
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the current price and the 20-period moving average, which may not be sufficient to capture the underlying trends and patterns in the market.
+*   The strategy does not account for volatility, which can lead to whipsaws and false signals.
+*   The strategy does not have a risk management component, which can lead to significant losses during periods of high market volatility.
+### Revised Strategy
+To improve the strategy, we can incorporate additional indicators and risk management techniques. Here's a revised strategy that uses a combination of moving averages and volatility to generate trading signals:
+*   We will use two moving averages with different time periods (short and long) to capture the trend and momentum.
+*   We will use the Bollinger Bands to account for volatility and avoid trading during periods of high volatility.
+*   We will use a risk management component to limit the number of trades and avoid over-leveraging.
+### Revised Python Strategy
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content="### Analysis of Weaknesses in the Strategy
+The given strategy uses two moving averages (MA) with window sizes of 50 and 200 to generate buy and sell signals. The strategy buys when the short MA crosses above the long MA and sells when the short MA crosses below the long MA. However, the backtest results show that the strategy did not make any trades, resulting in a 0% return.
+The weaknesses in the strategy are:
+* The MA window sizes may not be optimal for the 5-minute bar data.
+* The strategy only generates signals when the short MA crosses above or below the long MA, which may not be frequent enough to generate significant returns.
+* The strategy does not consider other market indicators or risk management techniques to optimize its performance.
+### Revised Strategy
+To improve the strategy, we can use a combination of MA and Relative Strength Index (RSI) to generate buy and sell signals. The RSI is a momentum indicator that measures the magnitude of recent price changes to determine overbought or oversold conditions.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">content='### Analysis of Weaknesses in the Strategy
+The given strategy uses a simple moving average crossover system, which can be improved in several ways:
+*   The strategy only considers the short and long moving averages, without taking into account other factors that might influence the stock price, such as volatility, trends, or momentum.
+*   The strategy uses a fixed window size for the short and long moving averages, which might not be optimal for all market conditions.
+*   The strategy does not have any risk management mechanisms, such as stop-loss or position sizing, which can help to limit losses and maximize gains.
+### Revised Strategy
+To improve the strategy, we can add a few more features:
+*   Use exponential moving averages (EMAs) instead of simple moving averages (SMAs), as EMAs give more weight to recent prices and can react faster to changes in the market.
+*   Add a volatility filter to avoid trading during periods of high volatility.
+*   Use a momentum indicator, such as the Relative Strength Index (RSI), to confirm the trading signals.
+Here is the revised strategy:
 </t>
   </si>
   <si>
@@ -422,6 +676,528 @@
     df.loc[df['signal'] != 0, 'position_size'] = pd.Series(10000 / df['hv'], index=df.index)  # Assuming $10,000 initial capital
     # Ensure signal Series uses the same index as df
     df["signal"] = pd.Series(df["signal"].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a context-aware mean reversion strategy.
+    Parameters:
+    - df (pd.DataFrame): Input DataFrame with OHLCV data.
+    Returns:
+    - None (modifies the input DataFrame in-place).
+    """
+    # Calculate Simple Moving Average (SMA) over 20 periods
+    df['sma_20'] = df['Close'].rolling(window=20).mean()
+    # Calculate Bollinger Bands (20-period SMA, 2-standard deviation)
+    df['bb_upper'] = df['sma_20'] + 2 * df['Close'].rolling(window=20).std()
+    df['bb_lower'] = df['sma_20'] - 2 * df['Close'].rolling(window=20).std()
+    # Calculate Average True Range (ATR) for risk management
+    df['hl'] = df['High'] - df['Low']
+    df['hc'] = np.abs(df['High'] - df['Close'].shift(1))
+    df['lc'] = np.abs(df['Low'] - df['Close'].shift(1))
+    df['tr'] = df[['hl', 'hc', 'lc']].max(axis=1)
+    df['atr'] = df['tr'].rolling(window=20).mean()
+    # Broad Market Trend Filter (using a 50-period SMA)
+    df['sma_50'] = df['Close'].rolling(window=50).mean()
+    market_trend = df['sma_20'] &gt; df['sma_50']
+    # Volatility Filter (avoid trading during high-volatility periods)
+    volatility_threshold = df['atr'].mean() * 1.5
+    low_volatility = df['atr'] &lt; volatility_threshold
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = 0
+    # Set Buy (1) when:
+    # - Below lower Bollinger Band
+    # - Market trend is upwards
+    # - Volatility is relatively low
+    buy_conditions = (df['Close'] &lt; df['bb_lower']) &amp; market_trend &amp; low_volatility
+    df.loc[buy_conditions, 'signal'] = 1
+    # Set Sell (-1) when:
+    # - Above upper Bollinger Band
+    # - Market trend is downwards
+    # - Volatility is relatively low
+    sell_conditions = (df['Close'] &gt; df['bb_upper']) &amp; ~market_trend &amp; low_volatility
+    df.loc[sell_conditions, 'signal'] = -1
+    # Basic Risk Management: Position Sizing based on ATR
+    df['position_size'] = 10000 / df['atr']  # Assuming $10,000 initial capital
+    # Ensure signal Series uses the same index as df
+    df["signal"] = pd.Series(df["signal"].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the input DataFrame based on a dual SMA strategy
+    with volatility-based position sizing.
+    """
+    # Calculate Short and Long Simple Moving Averages (SMA)
+    df['sma_short'] = df['Close'].rolling(window=10).mean()
+    df['sma_long'] = df['Close'].rolling(window=20).mean()
+    # Calculate Historical Volatility (HV) for position sizing
+    df['hv'] = df['Close'].rolling(window=20).std() * np.sqrt(5)  # 5-minute bars, scaled to daily HV
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = pd.Series(0, index=df.index)
+    # Set Buy (1) when Short SMA crosses above Long SMA and HV is below median
+    buy_conditions = (df['sma_short'] &gt; df['sma_long']) &amp; (df['hv'] &lt; df['hv'].median())
+    df.loc[buy_conditions, 'signal'] = 1
+    # Set Sell (-1) when Short SMA crosses below Long SMA or HV exceeds 1.5*median
+    sell_conditions = (df['sma_short'] &lt; df['sma_long']) | (df['hv'] &gt; 1.5 * df['hv'].median())
+    df.loc[sell_conditions, 'signal'] = -1
+    # Basic Volatility-Based Position Sizing (example: reduce position size with increasing HV)
+    df['position_size'] = pd.Series(1.0, index=df.index)  # default 100% size
+    df.loc[df['hv'] &gt; 1.5 * df['hv'].median(), 'position_size'] = 0.5  # reduce to 50% size when HV is high
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Calculate Short-term and Long-term Simple Moving Averages
+    df['sma_short'] = df['Close'].rolling(window=10).mean()
+    df['sma_long'] = df['Close'].rolling(window=30).mean()
+    # Calculate volatility (20-period Average True Range)
+    df['atr'] = df['High'].rolling(window=20).max() - df['Low'].rolling(window=20).min()
+    df['atr'] = df['atr'].rolling(window=20).mean()
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = 0
+    # Set Buy (1) when Short SMA crosses above Long SMA and price is not excessively high
+    buy_condition = (df['sma_short'] &gt; df['sma_long']) &amp; (df['Close'] &lt; df['sma_long'] * 1.02)
+    df.loc[buy_condition, 'signal'] = 1
+    # Set Sell (-1) when Short SMA crosses below Long SMA or stop-loss/profit conditions are met
+    sell_condition = (df['sma_short'] &lt; df['sma_long']) | \
+                     ((df['signal'].shift(1) == 1) &amp; ((df['Low'] &lt; (df['Close'].shift(1) - 2*df['atr'].shift(1))) | (df['High'] &gt; (df['Close'].shift(1) * 1.05))))
+    df.loc[sell_condition, 'signal'] = -1
+    # Ensure signal Series uses the same index as df
+    df["signal"] = pd.Series(df["signal"].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Calculate Simple Moving Average (SMA) over 20 periods
+    df['sma_20'] = df['Close'].rolling(window=20).mean()
+    # Calculate percentage difference between Close and SMA
+    df['pct_diff'] = ((df['Close'] - df['sma_20']) / df['sma_20']) * 100
+    # Calculate Relative Strength Index (RSI) over 10 periods for momentum confirmation
+    delta = df['Close'].diff(1)
+    up, down = delta.copy(), delta.copy()
+    up[up &lt; 0] = 0
+    down[down &gt; 0] = 0
+    roll_up = up.rolling(window=10).mean()
+    roll_down = down.rolling(window=10).mean().abs()
+    df['rsi'] = 100.0 - (100.0 / (1.0 + roll_up / roll_down))
+    # Calculate Average True Range (ATR) over 10 periods for risk management
+    high_low = df['High'] - df['Low']
+    high_close = np.abs(df['High'] - df['Close'].shift(1))
+    low_close = np.abs(df['Low'] - df['Close'].shift(1))
+    ranges = pd.concat([high_low, high_close, low_close], axis=1)
+    df['atr'] = ranges.max(axis=1).rolling(window=10).mean()
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = 0
+    # Set Buy (1) when:
+    # - Close is more than 1.5% below SMA
+    # - RSI is below 30 (oversold)
+    # - Position size is capped at 2% of portfolio based on ATR
+    buy_condition = (df['pct_diff'] &lt; -1.5) &amp; (df['rsi'] &lt; 30)
+    df.loc[buy_condition, 'signal'] = 1
+    df.loc[buy_condition, 'position_size'] = 0.02 / df['atr']
+    # Set Sell (-1) when:
+    # - Close is more than 1.5% above SMA
+    # - RSI is above 70 (overbought)
+    sell_condition = (df['pct_diff'] &gt; 1.5) &amp; (df['rsi'] &gt; 70)
+    df.loc[sell_condition, 'signal'] = -1
+    df.loc[sell_condition, 'position_size'] = 0.02 / df['atr']
+    # Ensure signal Series uses the same index as df
+    df["signal"] = pd.Series(df["signal"].values, index=df.index)
+    df["position_size"] = pd.Series(df["position_size"].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the input DataFrame based on a dual SMA strategy
+    with volatility-based position sizing.
+    """
+    # Calculate Short and Long Simple Moving Averages (SMA)
+    df['sma_short'] = df['Close'].rolling(window=10).mean()
+    df['sma_long'] = df['Close'].rolling(window=20).mean()
+    # Calculate Historical Volatility (HV) for position sizing
+    df['hv'] = df['Close'].rolling(window=20).std() * np.sqrt(5*60)  # 5-minute bars, 60 minutes/hour
+    # Initialize signal column with Hold (0) as default
+    df['signal'] = 0
+    # Set Buy (1) when Short SMA crosses above Long SMA and HV is below average
+    buy_cond = (df['sma_short'] &gt; df['sma_long']) &amp; (df['hv'] &lt; df['hv'].mean())
+    df.loc[buy_cond, 'signal'] = 1
+    # Set Sell (-1) when Short SMA crosses below Long SMA or HV exceeds 1.5*average
+    sell_cond = (df['sma_short'] &lt; df['sma_long']) | (df['hv'] &gt; 1.5*df['hv'].mean())
+    df.loc[sell_cond, 'signal'] = -1
+    # Basic Volatility-Based Position Sizing (inverse of HV)
+    df['position_size'] = pd.Series(1 / (1 + df['hv']), index=df.index)
+    # Ensure signal Series uses the same index as df
+    df['signal'] = pd.Series(df['signal'].values, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Calculate Simple Moving Average (SMA) over 20 periods
+    df['sma'] = df['Close'].rolling(window=20).mean()
+    # Calculate Adaptive Standard Deviation Multiplier (ASM) based on recent volatility
+    df['atr'] = df['High'].rolling(window=20).max() - df['Low'].rolling(window=20).min()
+    df['volatility_ratio'] = df['atr'] / df['Close']
+    df['asm'] = np.where(df['volatility_ratio'] &gt; 0.02, 1.5, np.where(df['volatility_ratio'] &lt; 0.01, 2.5, 2))
+    # Calculate Adaptive Bollinger Bands
+    df['std_dev'] = df['Close'].rolling(window=20).std()
+    df['lower_bb'] = df['sma'] - df['asm'] * df['std_dev']
+    df['upper_bb'] = df['sma'] + df['asm'] * df['std_dev']
+    # Initialize signal column with Hold (0) by default
+    df['signal'] = pd.Series(0, index=df.index)
+    # Generate Buy signal (1) when Close price crosses below Lower BB
+    buy_conditions = (df['Close'] &lt; df['lower_bb']) &amp; (df['Close'].shift(1) &gt;= df['lower_bb'].shift(1))
+    df.loc[buy_conditions, 'signal'] = 1
+    # Generate Sell signal (-1) when Close price crosses above Upper BB
+    sell_conditions = (df['Close'] &gt; df['upper_bb']) &amp; (df['Close'].shift(1) &lt;= df['upper_bb'].shift(1))
+    df.loc[sell_conditions, 'signal'] = -1
+    # Basic Risk Management: Position Sizing based on ATR (2% of equity per trade)
+    df['position_size'] = pd.Series(0, index=df.index)
+    df.loc[df['signal'] != 0, 'position_size'] = 0.02 * 10000 / df['atr']
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Calculate RSI
+    delta = df['Close'].diff(1)
+    up_days = delta.copy()
+    up_days[delta &lt;= 0] = 0
+    down_days = delta.copy()
+    down_days[delta &gt; 0] = 0
+    roll_up = up_days.rolling(window=14).mean()
+    roll_down = down_days.rolling(window=14).mean().abs()
+    RS = roll_up / roll_down
+    RSI = 100.0 - (100.0 / (1.0 + RS))
+    df['RSI'] = RSI
+    # Calculate Bollinger Bands
+    df['MA_20'] = df['Close'].rolling(window=20).mean()
+    df['Upper_BB'] = df['MA_20'] + 2*df['Close'].rolling(window=20).std()
+    df['Lower_BB'] = df['MA_20'] - 2*df['Close'].rolling(window=20).std()
+    # Generate buy and sell signals
+    buy_signals = np.where((df['RSI'] &lt; 30) &amp; (df['Close'] &lt; df['Lower_BB']), 1, 0)
+    sell_signals = np.where((df['RSI'] &gt; 70) &amp; (df['Close'] &gt; df['Upper_BB']), -1, 0)
+    signals = np.where(buy_signals == 1, 1, np.where(sell_signals == -1, -1, 0))
+    # Assign signals to the DataFrame
+    df["signal"] = pd.Series(signals, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a moving average crossover strategy with RSI.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame with OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate the short and long moving averages
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    # Calculate the Relative Strength Index (RSI)
+    delta = df['Close'].diff(1)
+    gain, loss = delta.copy(), delta.copy()
+    gain[gain &lt; 0] = 0
+    loss[loss &gt; 0] = 0
+    avg_gain = gain.rolling(window=14).mean()
+    avg_loss = abs(loss).rolling(window=14).mean()
+    rs = avg_gain / avg_loss
+    df['rsi'] = 100 - (100 / (1 + rs))
+    # Generate buy and sell signals
+    buy_signal = (df['short_ma'] &gt; df['long_ma']) &amp; (df['rsi'] &lt; 30)
+    sell_signal = (df['short_ma'] &lt; df['long_ma']) &amp; (df['rsi'] &gt; 70)
+    # Create the 'signal' column
+    signal = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    df['signal'] = pd.Series(signal, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a revised trading strategy.
+    The strategy uses exponential moving averages (EMAs) and the Relative Strength Index (RSI)
+    to generate buy and sell signals. It also includes a risk management mechanism to limit losses.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame containing the OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate exponential moving averages (EMAs)
+    short_window = 20
+    long_window = 50
+    df['short_ema'] = df['Close'].ewm(span=short_window, adjust=False).mean()
+    df['long_ema'] = df['Close'].ewm(span=long_window, adjust=False).mean()
+    # Calculate Relative Strength Index (RSI)
+    window = 14
+    delta = df['Close'].diff(1)
+    up, down = delta.copy(), delta.copy()
+    up[up &lt; 0] = 0
+    down[down &gt; 0] = 0
+    roll_up = up.ewm(com=window-1, adjust=False).mean()
+    roll_down = down.ewm(com=window-1, adjust=False).mean().abs()
+    RS = roll_up / roll_down
+    RSI = 100.0 - (100.0 / (1.0 + RS))
+    df['RSI'] = RSI
+    # Generate buy and sell signals
+    buy_signal = (df['Close'] &gt; df['short_ema']) &amp; (df['RSI'] &lt; 70)
+    sell_signal = (df['Close'] &lt; df['long_ema']) &amp; (df['RSI'] &gt; 30)
+    df['signal'] = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    # Add a risk management mechanism (stop-loss)
+    stop_loss = 0.02  # 2% stop-loss
+    df['stop_loss'] = df['Close'] * (1 - stop_loss)
+    df.loc[df['signal'] == 1, 'stop_loss'] = df['Close']
+    df['signal'] = np.where(df['Close'] &lt; df['stop_loss'], -1, df['signal'])
+    # Ensure the signal Series has the same index as the DataFrame
+    df['signal'] = pd.Series(df['signal'].values, index=df.index)
+# Example usage:
+df = pd.DataFrame({
+    'Open': [100, 101, 102, 103, 104],
+    'High': [105, 106, 107, 108, 109],
+    'Low': [95, 96, 97, 98, 99],
+    'Close': [100, 101, 102, 103, 104],
+    'Volume': [1000, 2000, 3000, 4000, 5000]
+})
+add_signal(df)
+print(df)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a moving average crossover strategy with risk management.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame with OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate short and long moving averages
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    # Calculate Average True Range (ATR)
+    high_low = df['High'] - df['Low']
+    high_close = (df['High'] - df['Close'].shift(1)).abs()
+    low_close = (df['Low'] - df['Close'].shift(1)).abs()
+    ranges = pd.concat([high_low, high_close, low_close], axis=1)
+    df['atr'] = ranges.max(axis=1).rolling(window=14).mean()
+    # Generate buy and sell signals based on moving average crossover and ATR
+    df['signal'] = np.where((df['Close'] &gt; df['short_ma']) &amp; (df['short_ma'] &gt; df['long_ma']) &amp; (df['atr'] &lt; df['Close'] * 0.02), 1, 
+                            np.where((df['Close'] &lt; df['short_ma']) &amp; (df['short_ma'] &lt; df['long_ma']) &amp; (df['atr'] &lt; df['Close'] * 0.02), -1, 0))
+    # Ensure the 'signal' Series has the same index as the DataFrame
+    df['signal'] = pd.Series(df['signal'].values, index=df.index)
+# Example usage:
+df = pd.DataFrame({
+    'Open': [100, 101, 102, 103, 104],
+    'High': [105, 106, 107, 108, 109],
+    'Low': [95, 96, 97, 98, 99],
+    'Close': [100, 101, 102, 103, 104],
+    'Volume': [1000, 2000, 3000, 4000, 5000]
+})
+add_signal(df)
+print(df)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a revised trading strategy.
+    The strategy uses a combination of short and long moving averages, as well as the Relative Strength Index (RSI).
+    It generates a buy signal when the short MA crosses above the long MA and the RSI is below 30 (oversold).
+    It generates a sell signal when the short MA crosses below the long MA and the RSI is above 70 (overbought).
+    """
+    # Calculate short and long moving averages
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    # Calculate Relative Strength Index (RSI)
+    delta = df['Close'].diff(1)
+    up, down = delta.copy(), delta.copy()
+    up[up &lt; 0] = 0
+    down[down &gt; 0] = 0
+    roll_up = up.rolling(window=14).mean()
+    roll_down = down.rolling(window=14).mean().abs()
+    RS = roll_up / roll_down
+    df['RSI'] = 100.0 - (100.0 / (1.0 + RS))
+    # Generate trading signals
+    df['signal'] = np.where((df['short_ma'] &gt; df['long_ma']) &amp; (df['RSI'] &lt; 30), 1, 
+                            np.where((df['short_ma'] &lt; df['long_ma']) &amp; (df['RSI'] &gt; 70), -1, 0))
+    # Ensure the signal Series has the same index as the DataFrame
+    df['signal'] = pd.Series(df['signal'].values, index=df.index)
+# Example usage
+df = pd.DataFrame({
+    'Open': [100, 101, 102, 103, 104],
+    'High': [105, 106, 107, 108, 109],
+    'Low': [95, 96, 97, 98, 99],
+    'Close': [100, 101, 102, 103, 104],
+    'Volume': [1000, 2000, 3000, 4000, 5000]
+})
+add_signal(df)
+print(df)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a revised moving average crossover strategy
+    that incorporates Bollinger Bands for volatility management.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame containing OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate the short and long moving averages
+    df['MA_10'] = df['Close'].rolling(window=10).mean()
+    df['MA_20'] = df['Close'].rolling(window=20).mean()
+    # Calculate the Bollinger Bands
+    df['BB_Middle'] = df['Close'].rolling(window=20).mean()
+    df['BB_Upper'] = df['BB_Middle'] + 2 * df['Close'].rolling(window=20).std()
+    df['BB_Lower'] = df['BB_Middle'] - 2 * df['Close'].rolling(window=20).std()
+    # Generate trading signals based on the moving average crossover and Bollinger Bands
+    buy_signal = (df['MA_10'] &gt; df['MA_20']) &amp; (df['Close'] &lt; df['BB_Lower'])
+    sell_signal = (df['MA_10'] &lt; df['MA_20']) &amp; (df['Close'] &gt; df['BB_Upper'])
+    # Create the 'signal' column
+    signal_array = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    df['signal'] = pd.Series(signal_array, index=df.index)
+# Example usage:
+# df = pd.read_csv('tsla_data.csv')
+# add_signal(df)
+# print(df.head())
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    # Calculate short and long MA
+    df['short_ma'] = df['Close'].rolling(window=20).mean()
+    df['long_ma'] = df['Close'].rolling(window=50).mean()
+    # Calculate RSI
+    delta = df['Close'].diff()
+    up, down = delta.copy(), delta.copy()
+    up[up &lt; 0] = 0
+    down[down &gt; 0] = 0
+    roll_up = up.rolling(window=14).mean()
+    roll_down = down.rolling(window=14).mean().abs()
+    RS = roll_up / roll_down
+    df['rsi'] = 100.0 - (100.0 / (1.0 + RS))
+    # Generate buy and sell signals
+    buy_signal = (df['short_ma'] &gt; df['long_ma']) &amp; (df['rsi'] &lt; 30)
+    sell_signal = (df['short_ma'] &lt; df['long_ma']) &amp; (df['rsi'] &gt; 70)
+    # Create signal column
+    signal_array = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    df['signal'] = pd.Series(signal_array, index=df.index)
+    return df
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a combination of moving averages and ATR.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame with OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate short and long moving averages
+    short_window = 20
+    long_window = 50
+    df['short_ma'] = df['Close'].rolling(window=short_window).mean()
+    df['long_ma'] = df['Close'].rolling(window=long_window).mean()
+    # Calculate Average True Range (ATR)
+    high_low = df['High'] - df['Low']
+    high_close = (df['High'] - df['Close'].shift(1)).abs()
+    low_close = (df['Low'] - df['Close'].shift(1)).abs()
+    ranges = pd.concat([high_low, high_close, low_close], axis=1)
+    df['atr'] = ranges.max(axis=1).rolling(window=14).mean()
+    # Generate signals based on moving average crossover and ATR
+    buy_signal = (df['Close'] &gt; df['short_ma']) &amp; (df['short_ma'] &gt; df['long_ma']) &amp; (df['atr'] &lt; df['atr'].rolling(window=20).mean())
+    sell_signal = (df['Close'] &lt; df['short_ma']) &amp; (df['short_ma'] &lt; df['long_ma']) &amp; (df['atr'] &gt; df['atr'].rolling(window=20).mean())
+    # Create the 'signal' column
+    signal = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    df['signal'] = pd.Series(signal, index=df.index)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+import pandas as pd
+import numpy as np
+def add_signal(df):
+    """
+    Adds a 'signal' column to the DataFrame based on a revised moving average crossover strategy.
+    Parameters:
+    df (pd.DataFrame): The input DataFrame containing the OHLCV data.
+    Returns:
+    None
+    """
+    # Calculate exponential moving averages
+    short_window = 20
+    long_window = 50
+    df['short_ema'] = df['Close'].ewm(span=short_window, adjust=False).mean()
+    df['long_ema'] = df['Close'].ewm(span=long_window, adjust=False).mean()
+    # Calculate Relative Strength Index (RSI)
+    delta = df['Close'].diff(1)
+    gain, loss = delta.copy(), delta.copy()
+    gain[gain &lt; 0] = 0
+    loss[loss &gt; 0] = 0
+    avg_gain = gain.ewm(span=14, adjust=False).mean()
+    avg_loss = loss.ewm(span=14, adjust=False).mean().abs()
+    rs = avg_gain / avg_loss
+    df['rsi'] = 100 - (100 / (1 + rs))
+    # Calculate volatility
+    df['volatility'] = df['Close'].rolling(window=20).std()
+    # Generate trading signals
+    buy_signal = (df['Close'] &gt; df['short_ema']) &amp; (df['short_ema'] &gt; df['long_ema']) &amp; (df['rsi'] &lt; 70) &amp; (df['volatility'] &lt; df['volatility'].mean())
+    sell_signal = (df['Close'] &lt; df['short_ema']) &amp; (df['short_ema'] &lt; df['long_ema']) &amp; (df['rsi'] &gt; 30) &amp; (df['volatility'] &lt; df['volatility'].mean())
+    hold_signal = ~(buy_signal | sell_signal)
+    # Assign signals to the 'signal' column
+    signal_array = np.where(buy_signal, 1, np.where(sell_signal, -1, 0))
+    df['signal'] = pd.Series(signal_array, index=df.index)
 </t>
   </si>
 </sst>
@@ -784,13 +1560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,22 +1651,28 @@
       <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:30">
       <c r="A2" s="2">
         <v>45787.60035719907</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="J2">
         <v>-0.71</v>
@@ -923,21 +1705,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:30">
       <c r="A3" s="2">
         <v>45787.64977077546</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="J3">
         <v>12.31</v>
@@ -976,21 +1758,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:30">
       <c r="A4" s="2">
         <v>45787.6773174074</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1029,21 +1811,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:30">
       <c r="A5" s="2">
         <v>45787.68231012731</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1082,21 +1864,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:30">
       <c r="A6" s="2">
-        <v>45787.68987413317</v>
+        <v>45787.68987413195</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="J6">
         <v>12.31</v>
@@ -1148,6 +1930,996 @@
       </c>
       <c r="AB6">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="2">
+        <v>45787.69154262731</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7">
+        <v>12.31</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>80</v>
+      </c>
+      <c r="M7">
+        <v>10000</v>
+      </c>
+      <c r="N7">
+        <v>9994.5</v>
+      </c>
+      <c r="O7">
+        <v>2.96</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>60</v>
+      </c>
+      <c r="R7">
+        <v>10000</v>
+      </c>
+      <c r="S7">
+        <v>9951.42</v>
+      </c>
+      <c r="V7">
+        <v>-0.06</v>
+      </c>
+      <c r="W7">
+        <v>0.49</v>
+      </c>
+      <c r="X7">
+        <v>-0.49</v>
+      </c>
+      <c r="Y7">
+        <v>0.6</v>
+      </c>
+      <c r="Z7">
+        <v>20</v>
+      </c>
+      <c r="AA7">
+        <v>20</v>
+      </c>
+      <c r="AB7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="2">
+        <v>45787.69203042824</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <v>12.31</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>80</v>
+      </c>
+      <c r="M8">
+        <v>10000</v>
+      </c>
+      <c r="N8">
+        <v>9994.5</v>
+      </c>
+      <c r="O8">
+        <v>-17.84</v>
+      </c>
+      <c r="P8">
+        <v>9</v>
+      </c>
+      <c r="Q8">
+        <v>90</v>
+      </c>
+      <c r="R8">
+        <v>10000</v>
+      </c>
+      <c r="S8">
+        <v>9705.58</v>
+      </c>
+      <c r="V8">
+        <v>-0.06</v>
+      </c>
+      <c r="W8">
+        <v>0.49</v>
+      </c>
+      <c r="X8">
+        <v>-2.94</v>
+      </c>
+      <c r="Y8">
+        <v>3.28</v>
+      </c>
+      <c r="Z8">
+        <v>10</v>
+      </c>
+      <c r="AA8">
+        <v>20</v>
+      </c>
+      <c r="AB8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="2">
+        <v>45787.69264355324</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9">
+        <v>12.31</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>80</v>
+      </c>
+      <c r="M9">
+        <v>10000</v>
+      </c>
+      <c r="N9">
+        <v>9994.5</v>
+      </c>
+      <c r="O9">
+        <v>-23</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>70</v>
+      </c>
+      <c r="R9">
+        <v>10000</v>
+      </c>
+      <c r="S9">
+        <v>9637.01</v>
+      </c>
+      <c r="V9">
+        <v>-0.06</v>
+      </c>
+      <c r="W9">
+        <v>0.49</v>
+      </c>
+      <c r="X9">
+        <v>-3.63</v>
+      </c>
+      <c r="Y9">
+        <v>4.29</v>
+      </c>
+      <c r="Z9">
+        <v>10</v>
+      </c>
+      <c r="AA9">
+        <v>30</v>
+      </c>
+      <c r="AB9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="2">
+        <v>45787.69377305556</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10">
+        <v>12.31</v>
+      </c>
+      <c r="K10">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>80</v>
+      </c>
+      <c r="M10">
+        <v>10000</v>
+      </c>
+      <c r="N10">
+        <v>9994.5</v>
+      </c>
+      <c r="O10">
+        <v>12.31</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="Q10">
+        <v>80</v>
+      </c>
+      <c r="R10">
+        <v>10000</v>
+      </c>
+      <c r="S10">
+        <v>9994.5</v>
+      </c>
+      <c r="V10">
+        <v>-0.06</v>
+      </c>
+      <c r="W10">
+        <v>0.49</v>
+      </c>
+      <c r="X10">
+        <v>-0.06</v>
+      </c>
+      <c r="Y10">
+        <v>0.49</v>
+      </c>
+      <c r="Z10">
+        <v>20</v>
+      </c>
+      <c r="AA10">
+        <v>10</v>
+      </c>
+      <c r="AB10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="2">
+        <v>45787.6947172338</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11">
+        <v>12.31</v>
+      </c>
+      <c r="K11">
+        <v>8</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+      <c r="M11">
+        <v>10000</v>
+      </c>
+      <c r="N11">
+        <v>9994.5</v>
+      </c>
+      <c r="O11">
+        <v>-20.88</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="Q11">
+        <v>90</v>
+      </c>
+      <c r="R11">
+        <v>10000</v>
+      </c>
+      <c r="S11">
+        <v>9641.440000000001</v>
+      </c>
+      <c r="V11">
+        <v>-0.06</v>
+      </c>
+      <c r="W11">
+        <v>0.49</v>
+      </c>
+      <c r="X11">
+        <v>-3.59</v>
+      </c>
+      <c r="Y11">
+        <v>4.26</v>
+      </c>
+      <c r="Z11">
+        <v>10</v>
+      </c>
+      <c r="AA11">
+        <v>20</v>
+      </c>
+      <c r="AB11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="2">
+        <v>45787.69563842592</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12">
+        <v>-0.62</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>80</v>
+      </c>
+      <c r="M12">
+        <v>10000</v>
+      </c>
+      <c r="N12">
+        <v>9917.83</v>
+      </c>
+      <c r="O12">
+        <v>-16.1</v>
+      </c>
+      <c r="P12">
+        <v>6</v>
+      </c>
+      <c r="Q12">
+        <v>60</v>
+      </c>
+      <c r="R12">
+        <v>10000</v>
+      </c>
+      <c r="S12">
+        <v>9870.33</v>
+      </c>
+      <c r="V12">
+        <v>-0.82</v>
+      </c>
+      <c r="W12">
+        <v>0.29</v>
+      </c>
+      <c r="X12">
+        <v>-1.3</v>
+      </c>
+      <c r="Y12">
+        <v>0.85</v>
+      </c>
+      <c r="Z12">
+        <v>20</v>
+      </c>
+      <c r="AA12">
+        <v>20</v>
+      </c>
+      <c r="AB12">
+        <v>20</v>
+      </c>
+      <c r="AC12">
+        <v>20</v>
+      </c>
+      <c r="AD12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="2">
+        <v>45787.69788519676</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13">
+        <v>0.88</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>40</v>
+      </c>
+      <c r="M13">
+        <v>10000</v>
+      </c>
+      <c r="N13">
+        <v>9966.98</v>
+      </c>
+      <c r="O13">
+        <v>-4.25</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>60</v>
+      </c>
+      <c r="R13">
+        <v>10000</v>
+      </c>
+      <c r="S13">
+        <v>9921.379999999999</v>
+      </c>
+      <c r="V13">
+        <v>-0.33</v>
+      </c>
+      <c r="W13">
+        <v>1.49</v>
+      </c>
+      <c r="X13">
+        <v>-0.79</v>
+      </c>
+      <c r="Y13">
+        <v>0.6</v>
+      </c>
+      <c r="Z13">
+        <v>14</v>
+      </c>
+      <c r="AA13">
+        <v>14</v>
+      </c>
+      <c r="AB13">
+        <v>20</v>
+      </c>
+      <c r="AC13">
+        <v>20</v>
+      </c>
+      <c r="AD13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="2">
+        <v>45787.70019128472</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14">
+        <v>-5.84</v>
+      </c>
+      <c r="K14">
+        <v>9</v>
+      </c>
+      <c r="L14">
+        <v>90</v>
+      </c>
+      <c r="M14">
+        <v>10000</v>
+      </c>
+      <c r="N14">
+        <v>9832.6</v>
+      </c>
+      <c r="O14">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>40</v>
+      </c>
+      <c r="R14">
+        <v>10000</v>
+      </c>
+      <c r="S14">
+        <v>10007.4</v>
+      </c>
+      <c r="V14">
+        <v>-1.67</v>
+      </c>
+      <c r="W14">
+        <v>2.98</v>
+      </c>
+      <c r="X14">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="Y14">
+        <v>0.61</v>
+      </c>
+      <c r="Z14">
+        <v>14</v>
+      </c>
+      <c r="AA14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="2">
+        <v>45787.7006875463</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15">
+        <v>-5.84</v>
+      </c>
+      <c r="K15">
+        <v>9</v>
+      </c>
+      <c r="L15">
+        <v>90</v>
+      </c>
+      <c r="M15">
+        <v>10000</v>
+      </c>
+      <c r="N15">
+        <v>9832.6</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>10000</v>
+      </c>
+      <c r="S15">
+        <v>10000</v>
+      </c>
+      <c r="V15">
+        <v>-1.67</v>
+      </c>
+      <c r="W15">
+        <v>2.98</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="2">
+        <v>45787.70490516203</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16">
+        <v>-5.84</v>
+      </c>
+      <c r="K16">
+        <v>9</v>
+      </c>
+      <c r="L16">
+        <v>90</v>
+      </c>
+      <c r="M16">
+        <v>10000</v>
+      </c>
+      <c r="N16">
+        <v>9832.6</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>10000</v>
+      </c>
+      <c r="S16">
+        <v>10000</v>
+      </c>
+      <c r="V16">
+        <v>-1.67</v>
+      </c>
+      <c r="W16">
+        <v>2.98</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="2">
+        <v>45787.70954210648</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17">
+        <v>-5.84</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17">
+        <v>90</v>
+      </c>
+      <c r="M17">
+        <v>10000</v>
+      </c>
+      <c r="N17">
+        <v>9832.6</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>10000</v>
+      </c>
+      <c r="S17">
+        <v>10000</v>
+      </c>
+      <c r="V17">
+        <v>-1.67</v>
+      </c>
+      <c r="W17">
+        <v>2.98</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>14</v>
+      </c>
+      <c r="AA17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="2">
+        <v>45787.71021422453</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18">
+        <v>1.51</v>
+      </c>
+      <c r="K18">
+        <v>9</v>
+      </c>
+      <c r="L18">
+        <v>90</v>
+      </c>
+      <c r="M18">
+        <v>10000</v>
+      </c>
+      <c r="N18">
+        <v>9928.540000000001</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>10000</v>
+      </c>
+      <c r="S18">
+        <v>10000</v>
+      </c>
+      <c r="V18">
+        <v>-0.71</v>
+      </c>
+      <c r="W18">
+        <v>2.04</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>10</v>
+      </c>
+      <c r="AA18">
+        <v>20</v>
+      </c>
+      <c r="AB18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="2">
+        <v>45787.71094487268</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>10000</v>
+      </c>
+      <c r="N19">
+        <v>10000</v>
+      </c>
+      <c r="O19">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19">
+        <v>40</v>
+      </c>
+      <c r="R19">
+        <v>10000</v>
+      </c>
+      <c r="S19">
+        <v>10007.4</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="Y19">
+        <v>0.61</v>
+      </c>
+      <c r="Z19">
+        <v>20</v>
+      </c>
+      <c r="AA19">
+        <v>50</v>
+      </c>
+      <c r="AB19">
+        <v>14</v>
+      </c>
+      <c r="AC19">
+        <v>50</v>
+      </c>
+      <c r="AD19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="2">
+        <v>45787.71153991898</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20">
+        <v>-5.84</v>
+      </c>
+      <c r="K20">
+        <v>9</v>
+      </c>
+      <c r="L20">
+        <v>90</v>
+      </c>
+      <c r="M20">
+        <v>10000</v>
+      </c>
+      <c r="N20">
+        <v>9832.6</v>
+      </c>
+      <c r="O20">
+        <v>-21.28</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>20</v>
+      </c>
+      <c r="R20">
+        <v>10000</v>
+      </c>
+      <c r="S20">
+        <v>9938.16</v>
+      </c>
+      <c r="V20">
+        <v>-1.67</v>
+      </c>
+      <c r="W20">
+        <v>2.98</v>
+      </c>
+      <c r="X20">
+        <v>-0.62</v>
+      </c>
+      <c r="Y20">
+        <v>0.42</v>
+      </c>
+      <c r="Z20">
+        <v>14</v>
+      </c>
+      <c r="AA20">
+        <v>20</v>
+      </c>
+      <c r="AB20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="2">
+        <v>45787.7119228124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21">
+        <v>-5.84</v>
+      </c>
+      <c r="K21">
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <v>90</v>
+      </c>
+      <c r="M21">
+        <v>10000</v>
+      </c>
+      <c r="N21">
+        <v>9832.6</v>
+      </c>
+      <c r="O21">
+        <v>-16.69</v>
+      </c>
+      <c r="P21">
+        <v>8</v>
+      </c>
+      <c r="Q21">
+        <v>80</v>
+      </c>
+      <c r="R21">
+        <v>10000</v>
+      </c>
+      <c r="S21">
+        <v>9790.459999999999</v>
+      </c>
+      <c r="V21">
+        <v>-1.67</v>
+      </c>
+      <c r="W21">
+        <v>2.98</v>
+      </c>
+      <c r="X21">
+        <v>-2.1</v>
+      </c>
+      <c r="Y21">
+        <v>1.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>